<commit_message>
✨expand to second version
</commit_message>
<xml_diff>
--- a/agenda.xlsx
+++ b/agenda.xlsx
@@ -1,73 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonesgranatyr/Documents/Ensino/IA Expert/Cursos/Assistente Virtual/curso_assistente/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A90D01-A057-1B44-8367-E035914D9D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="8620" yWindow="2220" windowWidth="15600" windowHeight="11320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>hora</t>
-  </si>
-  <si>
-    <t>descricao</t>
-  </si>
-  <si>
-    <t>responsavel</t>
-  </si>
-  <si>
-    <t>Reunião com a equipe de desenvolvimento</t>
-  </si>
-  <si>
-    <t>Reunião com o Call Center</t>
-  </si>
-  <si>
-    <t>Reunião com a Dell</t>
-  </si>
-  <si>
-    <t>João</t>
-  </si>
-  <si>
-    <t>Pedro</t>
-  </si>
-  <si>
-    <t>Maria</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+  <si>
+    <t xml:space="preserve">data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">descricao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">responsavel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reunião com a equipe de desenvolvimento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reunião com o Call Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">João</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reunião com a Dell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27-nov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Começo aula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inicio Python</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="d\-mmm"/>
+    <numFmt numFmtId="166" formatCode="h:mm"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -79,7 +106,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -87,186 +114,156 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="5">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="44546a"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="e7e6e6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="5b9bd5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="ed7d31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="a5a5a5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="ffc000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4472c4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="70ad47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0563c1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="954f72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
                 <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
                 <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
                 <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
                 <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
               </a:schemeClr>
@@ -274,33 +271,24 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
                 <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
@@ -313,13 +301,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -329,15 +311,13 @@
         <a:solidFill>
           <a:schemeClr val="phClr">
             <a:tint val="95000"/>
-            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
-                <a:satMod val="150000"/>
                 <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
@@ -345,7 +325,6 @@
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
-                <a:satMod val="130000"/>
                 <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
@@ -353,117 +332,139 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="63000"/>
-                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.67"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
         <v>44911</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2" t="n">
+        <v>0.729166666666667</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>44911</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>44911</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>44911</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="D4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>0.569444444444444</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="n">
         <v>0.75</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>44911</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>